<commit_message>
Ispravljene sitne greske u glavnom usecase i scenariju za registraciju
</commit_message>
<xml_diff>
--- a/UseCaseScenarij/Scenarij za registraciju i login.xlsx
+++ b/UseCaseScenarij/Scenarij za registraciju i login.xlsx
@@ -24,48 +24,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+  <si>
+    <t>1. Zahtjev za registraciju</t>
+  </si>
+  <si>
+    <t>2. Unos podataka za registraciju</t>
+  </si>
+  <si>
+    <t>8. Unos username-a i sifre za pristup sistemu</t>
+  </si>
+  <si>
+    <t>10. Pristup pocetnom interfejsu</t>
+  </si>
+  <si>
+    <t>3. Validacija podataka</t>
+  </si>
+  <si>
+    <t>4. Dodjela username-a</t>
+  </si>
+  <si>
+    <t>5. Kreiranje profila</t>
+  </si>
+  <si>
+    <t>7. Vracanje korisnika na login formu</t>
+  </si>
+  <si>
+    <t>9. Validacija unesenih podataka</t>
+  </si>
+  <si>
+    <t>6. Spasavanje u bazu</t>
+  </si>
   <si>
     <t>KORISNIK</t>
   </si>
   <si>
-    <t>SISTEM ZA REGISTRACIJU</t>
+    <t>SISTEM</t>
   </si>
   <si>
     <t>ADMIN</t>
   </si>
   <si>
-    <t>1. Zahtjev za registraciju</t>
-  </si>
-  <si>
-    <t>2. Unos podataka za registraciju</t>
-  </si>
-  <si>
-    <t>3. Validacija podataka</t>
-  </si>
-  <si>
-    <t>4. Dodjela username-a</t>
-  </si>
-  <si>
-    <t>5. Kreiranje profila</t>
-  </si>
-  <si>
-    <t>6. Unos u bazu</t>
-  </si>
-  <si>
-    <t>7. Vracanje korisnika na login formu</t>
-  </si>
-  <si>
-    <t>8. Unos username-a i sifre za pristup sistemu</t>
-  </si>
-  <si>
-    <t>9. Validacija unesenih podataka</t>
-  </si>
-  <si>
-    <t>10. Pristup pocetnom interfejsu</t>
-  </si>
-  <si>
-    <t>Alternativni tok dogadjaja. Preduvjet: podaci su pogresni prilikom registrovanja</t>
+    <t>Alternativni tok dogadjaja. Preduvjet: podaci su pogresni prilikom registrovanja.</t>
   </si>
   <si>
     <t>1. Prijava greske</t>
@@ -83,41 +83,56 @@
     <t>Alternativni tok dogadjaja. Preduvjet: korisnik je zaboravio sifru te ne moze pristupiti profilu</t>
   </si>
   <si>
-    <t>SISTEM ZA LOGIN</t>
+    <t>1. Zahtjev za password recovery</t>
+  </si>
+  <si>
+    <t>3. Verifikacija e-maila</t>
+  </si>
+  <si>
+    <t>4. Odabir nove sifre</t>
   </si>
   <si>
     <t>SISTEM ZA MAILOVE</t>
   </si>
   <si>
-    <t>1. Zahtjev za password recovery</t>
-  </si>
-  <si>
     <t>2. Slanje e-maila korisniku</t>
-  </si>
-  <si>
-    <t>3. Verifikacija e-maila</t>
-  </si>
-  <si>
-    <t>4. Odabir nove sifre</t>
-  </si>
-  <si>
-    <t>5. Azuriranje profila u bazi</t>
-  </si>
-  <si>
-    <t>6. Nastavak na korak 7. glavnog toka</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -140,10 +155,36 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -425,189 +466,200 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.7109375" customWidth="1"/>
-    <col min="2" max="2" width="37.7109375" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" customWidth="1"/>
+    <col min="1" max="1" width="37.28515625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="7"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B11" s="4"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="B15" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="C15" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
-        <v>2</v>
+      <c r="A19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+      <c r="A20" s="2"/>
+      <c r="B20" s="9" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+      <c r="A21" s="2"/>
+      <c r="B21" s="6" t="s">
         <v>17</v>
       </c>
     </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+    </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="A23" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="A24" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C24" t="s">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25"/>
+      <c r="C25" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A14:C14"/>
     <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A22:C22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>